<commit_message>
[*] Task 10 Before Added bias
</commit_message>
<xml_diff>
--- a/MyProjects/p74_Conveyor/result/neural_network_model/cases02.xlsx
+++ b/MyProjects/p74_Conveyor/result/neural_network_model/cases02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A\M\MyProjects\p74_Conveyor\result\neural_network_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A\Pro\M\MyProjects\p74_Conveyor\result\neural_network_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A220FE-1E56-443C-9E75-E3C406D8C3A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4761744A-1AA1-48C8-A494-082C836A0742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="28800" yWindow="1590" windowWidth="19200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Наименование</t>
   </si>
@@ -251,7 +251,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,26 +532,26 @@
   <dimension ref="A7:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.88671875" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" customWidth="1"/>
+    <col min="10" max="10" width="5.44140625" customWidth="1"/>
+    <col min="11" max="11" width="4.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
     <col min="13" max="13" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:16" ht="39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
@@ -580,7 +580,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -611,7 +611,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="10" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -653,7 +653,7 @@
       </c>
       <c r="N10" s="9"/>
     </row>
-    <row r="13" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -702,7 +702,7 @@
         <v>0.9066764306905899</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -746,7 +746,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>29</v>
       </c>
@@ -788,13 +788,16 @@
       </c>
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -833,7 +836,7 @@
       </c>
       <c r="N18" s="9"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -872,10 +875,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -916,7 +919,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -957,7 +960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -999,7 +1002,7 @@
       </c>
       <c r="N25" s="9"/>
     </row>
-    <row r="26" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L33" s="1"/>
     </row>
   </sheetData>

</xml_diff>